<commit_message>
return to main window when finish work
</commit_message>
<xml_diff>
--- a/test.xlsx
+++ b/test.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A2:B4"/>
+  <dimension ref="A2:B5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -457,6 +457,18 @@
         </is>
       </c>
     </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>awake</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>thức giấc</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
fix bug display image in fill word mode. Fix bug crash app when can not find image, translate word
</commit_message>
<xml_diff>
--- a/test.xlsx
+++ b/test.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A2:B5"/>
+  <dimension ref="A2:B8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -469,6 +469,42 @@
         </is>
       </c>
     </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>have</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>có</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>havaaa</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>havaaa</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>haw</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>ồ</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
display error message when create lesson. build new app to run
</commit_message>
<xml_diff>
--- a/test.xlsx
+++ b/test.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A2:B8"/>
+  <dimension ref="A2:B9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -505,6 +505,18 @@
         </is>
       </c>
     </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>happy</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>vui mừng</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>